<commit_message>
Finish calibrating PESMO CO + re-run ESTD CO 2021
</commit_message>
<xml_diff>
--- a/EnergyScope_Pathway_CO/src/resources.xlsx
+++ b/EnergyScope_Pathway_CO/src/resources.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C167"/>
+  <dimension ref="A1:C160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,77 +479,77 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>GASOLINE</t>
+          <t>ELECTRICITY</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>27857.13986825701</v>
+        <v>4.753708569349724</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n"/>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>DIESEL</t>
+          <t>GASOLINE</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>90750.49571856338</v>
+        <v>63438.0012783999</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>BIOETHANOL</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1504.900000059549</v>
+        <v>70949.00594103248</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>BIODIESEL</t>
+          <t>BIOETHANOL</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>4139.100000029775</v>
+        <v>6180.10350934952</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>LFO</t>
+          <t>BIODIESEL</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>76056.83905326828</v>
+        <v>2541.007064379375</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>GAS</t>
+          <t>LFO</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>44716.57222204022</v>
+        <v>40769.0087268369</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>GAS_RE</t>
+          <t>GAS</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>3.252838351779349e-07</v>
+        <v>89470.47792505349</v>
       </c>
     </row>
     <row r="9">
@@ -560,1780 +560,1703 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>6140.096733683597</v>
+        <v>31309.07398398421</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>WET_BIOMASS</t>
+          <t>COAL</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8365.50008298485</v>
+        <v>40990.00162601373</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>COAL</t>
+          <t>URANIUM</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>14107.66806055842</v>
+        <v>0.1167885569535576</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>URANIUM</t>
+          <t>ELEC_EXPORT</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>101167.4428728</v>
+        <v>-0.2700966439322485</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>WASTE</t>
+          <t>CO2_EMISSIONS</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3693.879986790369</v>
+        <v>32440.59165309996</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>H2</t>
+          <t>RES_WIND</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1.914026777286213e-06</v>
+        <v>2.349687443257729</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>H2_RE</t>
+          <t>RES_SOLAR</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>3.766386175144278e-07</v>
+        <v>220.6978388906463</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>AMMONIA</t>
+          <t>RES_HYDRO</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1.274997710088253e-05</v>
+        <v>60862.6483831542</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>AMMONIA_RE</t>
+          <t>CO2_ATM</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>7.365767366492628e-06</v>
+        <v>0.01300863514791514</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n"/>
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>YEAR_2025</t>
+        </is>
+      </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>METHANOL_RE</t>
+          <t>ELECTRICITY</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>5.327447579121103e-06</v>
+        <v>0.05196578578960023</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>ELEC_EXPORT</t>
+          <t>GASOLINE</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>5579.354364820338</v>
+        <v>47622.31585194236</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>CO2_EMISSIONS</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>18513.0292590365</v>
+        <v>70116.3392925895</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>RES_WIND</t>
+          <t>BIOETHANOL</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>12800.00000000892</v>
+        <v>0.01041102543020517</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>RES_SOLAR</t>
+          <t>BIODIESEL</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>5201.116792014252</v>
+        <v>0.01685436479194573</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>RES_HYDRO</t>
+          <t>LFO</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>38769.83173042576</v>
+        <v>44845.15104348576</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>CO2_ATM</t>
+          <t>GAS</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>3.415198886058606e-06</v>
+        <v>24591.10074638199</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="inlineStr">
-        <is>
-          <t>YEAR_2025</t>
-        </is>
-      </c>
+      <c r="A25" s="1" t="n"/>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>ELECTRICITY</t>
+          <t>GAS_RE</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1.119488739142686e-05</v>
+        <v>0.001505927542535378</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>GASOLINE</t>
+          <t>WOOD</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2400.232275029869</v>
+        <v>5269.872709672889</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>DIESEL</t>
+          <t>WET_BIOMASS</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>71223.49994576948</v>
+        <v>49632.51054439084</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n"/>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>BIOETHANOL</t>
+          <t>COAL</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>7.769233388243627e-06</v>
+        <v>45018.04000961654</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n"/>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>BIODIESEL</t>
+          <t>WASTE</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>6.429905467179617e-06</v>
+        <v>0.4008440470811172</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n"/>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>LFO</t>
+          <t>H2</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>54073.69905341577</v>
+        <v>0.007303991457372299</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n"/>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>GAS</t>
+          <t>H2_RE</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>42033.46795265877</v>
+        <v>0.002861065085895547</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n"/>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>GAS_RE</t>
+          <t>AMMONIA</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>3.379887573069996e-06</v>
+        <v>0.175073214808293</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n"/>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>WOOD</t>
+          <t>AMMONIA_RE</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>6111.637967275137</v>
+        <v>0.07843261531537699</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n"/>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>WET_BIOMASS</t>
+          <t>METHANOL</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>49632.65389495983</v>
+        <v>0.1007374882463438</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n"/>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>COAL</t>
+          <t>METHANOL_RE</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>45018.82708975715</v>
+        <v>0.03862752459387328</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n"/>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>WASTE</t>
+          <t>ELEC_EXPORT</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>340.9889188136733</v>
+        <v>0.1304201280930073</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n"/>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>H2</t>
+          <t>CO2_EMISSIONS</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>9.262880941943882e-07</v>
+        <v>37654.498067078</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n"/>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>H2_RE</t>
+          <t>RES_WIND</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>3.501493703202985e-07</v>
+        <v>2.526292782595421</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n"/>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>AMMONIA</t>
+          <t>RES_SOLAR</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>9.083246601617457e-06</v>
+        <v>38005.69180761097</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n"/>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>AMMONIA_RE</t>
+          <t>RES_HYDRO</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>7.900510943191133e-06</v>
+        <v>66970.71997652773</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n"/>
       <c r="B41" s="1" t="inlineStr">
         <is>
-          <t>METHANOL</t>
+          <t>RES_GEO</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1.736479400798633e-05</v>
+        <v>0.02922531910420124</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n"/>
       <c r="B42" s="1" t="inlineStr">
         <is>
-          <t>METHANOL_RE</t>
+          <t>CO2_ATM</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>6.637736883580071e-06</v>
+        <v>0.01241787915213161</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="n"/>
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>YEAR_2030</t>
+        </is>
+      </c>
       <c r="B43" s="1" t="inlineStr">
         <is>
-          <t>ELEC_EXPORT</t>
+          <t>ELECTRICITY</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>8.397950196581405e-06</v>
+        <v>0.04969531585438923</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n"/>
       <c r="B44" s="1" t="inlineStr">
         <is>
-          <t>CO2_EMISSIONS</t>
+          <t>GASOLINE</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>38152.29831973334</v>
+        <v>9559.931411273297</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n"/>
       <c r="B45" s="1" t="inlineStr">
         <is>
-          <t>RES_WIND</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>12799.99999251347</v>
+        <v>69014.24798594227</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n"/>
       <c r="B46" s="1" t="inlineStr">
         <is>
-          <t>RES_SOLAR</t>
+          <t>BIOETHANOL</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>20590.22283360128</v>
+        <v>0.04372017021756814</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n"/>
       <c r="B47" s="1" t="inlineStr">
         <is>
-          <t>RES_HYDRO</t>
+          <t>BIODIESEL</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>66970.63172764055</v>
+        <v>0.02247032789324637</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n"/>
       <c r="B48" s="1" t="inlineStr">
         <is>
-          <t>RES_GEO</t>
+          <t>LFO</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>4.90466251187802e-06</v>
+        <v>44979.70985971947</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n"/>
       <c r="B49" s="1" t="inlineStr">
         <is>
-          <t>CO2_ATM</t>
+          <t>GAS</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>2.396425993270941e-06</v>
+        <v>16855.19209929599</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="inlineStr">
-        <is>
-          <t>YEAR_2030</t>
-        </is>
-      </c>
+      <c r="A50" s="1" t="n"/>
       <c r="B50" s="1" t="inlineStr">
         <is>
-          <t>ELECTRICITY</t>
+          <t>GAS_RE</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1.047306211931322e-05</v>
+        <v>0.003503556286944329</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n"/>
       <c r="B51" s="1" t="inlineStr">
         <is>
-          <t>GASOLINE</t>
+          <t>WOOD</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1.704215142993256e-05</v>
+        <v>12026.83310655999</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n"/>
       <c r="B52" s="1" t="inlineStr">
         <is>
-          <t>DIESEL</t>
+          <t>WET_BIOMASS</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>48891.08642554688</v>
+        <v>49781.97283790607</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n"/>
       <c r="B53" s="1" t="inlineStr">
         <is>
-          <t>BIOETHANOL</t>
+          <t>COAL</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>7.780685944363176e-06</v>
+        <v>47111.58557564245</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n"/>
       <c r="B54" s="1" t="inlineStr">
         <is>
-          <t>BIODIESEL</t>
+          <t>WASTE</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1.008940376883334e-05</v>
+        <v>0.6700262364456991</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n"/>
       <c r="B55" s="1" t="inlineStr">
         <is>
-          <t>LFO</t>
+          <t>H2</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>44980.39573120538</v>
+        <v>0.01127781011387228</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n"/>
       <c r="B56" s="1" t="inlineStr">
         <is>
-          <t>GAS</t>
+          <t>H2_RE</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>35656.33469325991</v>
+        <v>0.00483679588913296</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n"/>
       <c r="B57" s="1" t="inlineStr">
         <is>
-          <t>GAS_RE</t>
+          <t>AMMONIA_RE</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>4.660301804411187e-07</v>
+        <v>0.1792535607685895</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n"/>
       <c r="B58" s="1" t="inlineStr">
         <is>
-          <t>WOOD</t>
+          <t>METHANOL</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>13289.87179476815</v>
+        <v>0.1122169291615862</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n"/>
       <c r="B59" s="1" t="inlineStr">
         <is>
-          <t>WET_BIOMASS</t>
+          <t>METHANOL_RE</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>49781.99998731168</v>
+        <v>0.06365269546988526</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n"/>
       <c r="B60" s="1" t="inlineStr">
         <is>
-          <t>COAL</t>
+          <t>ELEC_EXPORT</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>49293.63494893954</v>
+        <v>0.1362951008452598</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n"/>
       <c r="B61" s="1" t="inlineStr">
         <is>
-          <t>WASTE</t>
+          <t>CO2_EMISSIONS</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>0.0002222313902551923</v>
+        <v>40697.98800101976</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n"/>
       <c r="B62" s="1" t="inlineStr">
         <is>
-          <t>H2</t>
+          <t>RES_WIND</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>2.216875422040499e-06</v>
+        <v>2.744226898558167</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n"/>
       <c r="B63" s="1" t="inlineStr">
         <is>
-          <t>H2_RE</t>
+          <t>RES_SOLAR</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>6.59722074828153e-07</v>
+        <v>84728.87216335004</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n"/>
       <c r="B64" s="1" t="inlineStr">
         <is>
-          <t>AMMONIA_RE</t>
+          <t>RES_HYDRO</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1.724121194291841e-05</v>
+        <v>66970.70929550486</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n"/>
       <c r="B65" s="1" t="inlineStr">
         <is>
-          <t>METHANOL</t>
+          <t>RES_GEO</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>2.234630200282778e-05</v>
+        <v>0.0521540952351667</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n"/>
       <c r="B66" s="1" t="inlineStr">
         <is>
-          <t>METHANOL_RE</t>
+          <t>CO2_ATM</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1.182322673082081e-05</v>
+        <v>0.01856736816558213</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="n"/>
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>YEAR_2035</t>
+        </is>
+      </c>
       <c r="B67" s="1" t="inlineStr">
         <is>
-          <t>ELEC_EXPORT</t>
+          <t>ELECTRICITY</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1.338364759817523e-05</v>
+        <v>0.4388754404095259</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n"/>
       <c r="B68" s="1" t="inlineStr">
         <is>
-          <t>CO2_EMISSIONS</t>
+          <t>GASOLINE</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>41508.24818745329</v>
+        <v>0.08063320536891902</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n"/>
       <c r="B69" s="1" t="inlineStr">
         <is>
-          <t>RES_WIND</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>12799.99998607875</v>
+        <v>941.7599084687142</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n"/>
       <c r="B70" s="1" t="inlineStr">
         <is>
-          <t>RES_SOLAR</t>
+          <t>BIOETHANOL</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>64269.53736883542</v>
+        <v>0.02506079085736702</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n"/>
       <c r="B71" s="1" t="inlineStr">
         <is>
-          <t>RES_HYDRO</t>
+          <t>BIODIESEL</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>66970.63172581591</v>
+        <v>0.05157857463531269</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n"/>
       <c r="B72" s="1" t="inlineStr">
         <is>
-          <t>RES_GEO</t>
+          <t>LFO</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>9.022403257969446e-06</v>
+        <v>3.451698116679053</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n"/>
       <c r="B73" s="1" t="inlineStr">
         <is>
-          <t>CO2_ATM</t>
+          <t>GAS</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>3.13425080210373e-06</v>
+        <v>79143.76978138488</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="1" t="inlineStr">
-        <is>
-          <t>YEAR_2035</t>
-        </is>
-      </c>
+      <c r="A74" s="1" t="n"/>
       <c r="B74" s="1" t="inlineStr">
         <is>
-          <t>ELECTRICITY</t>
+          <t>GAS_RE</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0.3950074739497882</v>
+        <v>0.004189510537843146</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n"/>
       <c r="B75" s="1" t="inlineStr">
         <is>
-          <t>GASOLINE</t>
+          <t>WOOD</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>1.393371928993799e-05</v>
+        <v>74740.41635688637</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n"/>
       <c r="B76" s="1" t="inlineStr">
         <is>
-          <t>DIESEL</t>
+          <t>WET_BIOMASS</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>941.6502516040238</v>
+        <v>49781.99196996895</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n"/>
       <c r="B77" s="1" t="inlineStr">
         <is>
-          <t>BIOETHANOL</t>
+          <t>COAL</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>9.23749551295759e-06</v>
+        <v>45723.17436000186</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n"/>
       <c r="B78" s="1" t="inlineStr">
         <is>
-          <t>BIODIESEL</t>
+          <t>WASTE</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>1.739257263012072e-05</v>
+        <v>1.310724117264497</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n"/>
       <c r="B79" s="1" t="inlineStr">
         <is>
-          <t>LFO</t>
+          <t>H2</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>0.001036579360277805</v>
+        <v>0.006877017619992277</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n"/>
       <c r="B80" s="1" t="inlineStr">
         <is>
-          <t>GAS</t>
+          <t>H2_RE</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>59706.55253585739</v>
+        <v>0.004785331133980817</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n"/>
       <c r="B81" s="1" t="inlineStr">
         <is>
-          <t>GAS_RE</t>
+          <t>AMMONIA_RE</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>2.049911151514828e-06</v>
+        <v>0.06806569179367949</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n"/>
       <c r="B82" s="1" t="inlineStr">
         <is>
-          <t>WOOD</t>
+          <t>METHANOL</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>74744.35069647086</v>
+        <v>0.1087462660411594</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n"/>
       <c r="B83" s="1" t="inlineStr">
         <is>
-          <t>WET_BIOMASS</t>
+          <t>METHANOL_RE</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>49781.99998946534</v>
+        <v>0.07466035800227519</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n"/>
       <c r="B84" s="1" t="inlineStr">
         <is>
-          <t>COAL</t>
+          <t>ELEC_EXPORT</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>43533.27706751277</v>
+        <v>0.3911106181832409</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n"/>
       <c r="B85" s="1" t="inlineStr">
         <is>
-          <t>WASTE</t>
+          <t>CO2_EMISSIONS</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>0.0003349628941991568</v>
+        <v>53888.41427135409</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n"/>
       <c r="B86" s="1" t="inlineStr">
         <is>
-          <t>H2</t>
+          <t>RES_WIND</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>1.267421826300833e-06</v>
+        <v>3.197047222170045</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n"/>
       <c r="B87" s="1" t="inlineStr">
         <is>
-          <t>H2_RE</t>
+          <t>RES_SOLAR</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>7.151671390210986e-07</v>
+        <v>140406.0520345559</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n"/>
       <c r="B88" s="1" t="inlineStr">
         <is>
-          <t>AMMONIA_RE</t>
+          <t>RES_HYDRO</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>1.69653397433799e-05</v>
+        <v>66970.55812710227</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n"/>
       <c r="B89" s="1" t="inlineStr">
         <is>
-          <t>METHANOL</t>
+          <t>RES_GEO</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>2.002072837547172e-05</v>
+        <v>0.08287442969607033</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n"/>
       <c r="B90" s="1" t="inlineStr">
         <is>
-          <t>METHANOL_RE</t>
+          <t>CO2_ATM</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>1.523660233656918e-05</v>
+        <v>0.06731210487953634</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="1" t="n"/>
+      <c r="A91" s="1" t="inlineStr">
+        <is>
+          <t>YEAR_2040</t>
+        </is>
+      </c>
       <c r="B91" s="1" t="inlineStr">
         <is>
-          <t>ELEC_EXPORT</t>
+          <t>ELECTRICITY</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>3.660815787043248e-05</v>
+        <v>0.05748651972868573</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n"/>
       <c r="B92" s="1" t="inlineStr">
         <is>
-          <t>CO2_EMISSIONS</t>
+          <t>GASOLINE</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>53099.90210032007</v>
+        <v>0.1123598285795269</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n"/>
       <c r="B93" s="1" t="inlineStr">
         <is>
-          <t>RES_WIND</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>12799.99994537754</v>
+        <v>914.6631015863123</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n"/>
       <c r="B94" s="1" t="inlineStr">
         <is>
-          <t>RES_SOLAR</t>
+          <t>BIOETHANOL</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>132218.318970923</v>
+        <v>0.04750387262578974</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n"/>
       <c r="B95" s="1" t="inlineStr">
         <is>
-          <t>RES_HYDRO</t>
+          <t>BIODIESEL</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>66970.63168894265</v>
+        <v>0.1058414127350015</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n"/>
       <c r="B96" s="1" t="inlineStr">
         <is>
-          <t>RES_GEO</t>
+          <t>LFO</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>1.437885029992555e-05</v>
+        <v>1.668436169889619</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n"/>
       <c r="B97" s="1" t="inlineStr">
         <is>
-          <t>CO2_ATM</t>
+          <t>GAS</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>1.126180558237521e-05</v>
+        <v>72224.83644992554</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="1" t="inlineStr">
-        <is>
-          <t>YEAR_2040</t>
-        </is>
-      </c>
+      <c r="A98" s="1" t="n"/>
       <c r="B98" s="1" t="inlineStr">
         <is>
-          <t>ELECTRICITY</t>
+          <t>GAS_RE</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>1.189185338067959e-05</v>
+        <v>0.003861215305708258</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n"/>
       <c r="B99" s="1" t="inlineStr">
         <is>
-          <t>GASOLINE</t>
+          <t>WOOD</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>1.548484380884851e-05</v>
+        <v>75071.53539355769</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n"/>
       <c r="B100" s="1" t="inlineStr">
         <is>
-          <t>DIESEL</t>
+          <t>WET_BIOMASS</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>914.6240257681318</v>
+        <v>49781.99887370475</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n"/>
       <c r="B101" s="1" t="inlineStr">
         <is>
-          <t>BIOETHANOL</t>
+          <t>COAL</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>1.268855708780975e-05</v>
+        <v>28190.90972130801</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n"/>
       <c r="B102" s="1" t="inlineStr">
         <is>
-          <t>BIODIESEL</t>
+          <t>WASTE</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>2.892663236718488e-05</v>
+        <v>2.220129039347286</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n"/>
       <c r="B103" s="1" t="inlineStr">
         <is>
-          <t>LFO</t>
+          <t>H2</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>0.0003670425268564579</v>
+        <v>0.007043609002339978</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n"/>
       <c r="B104" s="1" t="inlineStr">
         <is>
-          <t>GAS</t>
+          <t>H2_RE</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>61841.80418535886</v>
+        <v>0.006293708081667796</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n"/>
       <c r="B105" s="1" t="inlineStr">
         <is>
-          <t>GAS_RE</t>
+          <t>AMMONIA_RE</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>5.26805012749933e-06</v>
+        <v>0.1267926363912942</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n"/>
       <c r="B106" s="1" t="inlineStr">
         <is>
-          <t>WOOD</t>
+          <t>METHANOL</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>75072.99987728833</v>
+        <v>0.1315207585316001</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n"/>
       <c r="B107" s="1" t="inlineStr">
         <is>
-          <t>WET_BIOMASS</t>
+          <t>METHANOL_RE</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>49781.99998550022</v>
+        <v>0.1186862288680828</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n"/>
       <c r="B108" s="1" t="inlineStr">
         <is>
-          <t>COAL</t>
+          <t>ELEC_EXPORT</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>35089.09349503346</v>
+        <v>0.4501271034173335</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n"/>
       <c r="B109" s="1" t="inlineStr">
         <is>
-          <t>WASTE</t>
+          <t>CO2_EMISSIONS</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>0.0005805645727654735</v>
+        <v>47217.06588709373</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n"/>
       <c r="B110" s="1" t="inlineStr">
         <is>
-          <t>H2</t>
+          <t>RES_WIND</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>1.273495841111937e-06</v>
+        <v>3.2972070140673</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n"/>
       <c r="B111" s="1" t="inlineStr">
         <is>
-          <t>H2_RE</t>
+          <t>RES_SOLAR</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>9.567386931416025e-07</v>
+        <v>175147.7580181581</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n"/>
       <c r="B112" s="1" t="inlineStr">
         <is>
-          <t>AMMONIA_RE</t>
+          <t>RES_HYDRO</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>2.246984715312102e-05</v>
+        <v>66970.61956606914</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n"/>
       <c r="B113" s="1" t="inlineStr">
         <is>
-          <t>METHANOL</t>
+          <t>RES_GEO</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>2.466443825058099e-05</v>
+        <v>0.1151540416508027</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n"/>
       <c r="B114" s="1" t="inlineStr">
         <is>
-          <t>METHANOL_RE</t>
+          <t>CO2_ATM</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>2.574046519321391e-05</v>
+        <v>0.1242945929567517</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="1" t="n"/>
+      <c r="A115" s="1" t="inlineStr">
+        <is>
+          <t>YEAR_2045</t>
+        </is>
+      </c>
       <c r="B115" s="1" t="inlineStr">
         <is>
-          <t>ELEC_EXPORT</t>
+          <t>ELECTRICITY</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>4.413263802405254e-05</v>
+        <v>0.06465790759771584</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n"/>
       <c r="B116" s="1" t="inlineStr">
         <is>
-          <t>CO2_EMISSIONS</t>
+          <t>GASOLINE</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>49699.35285994682</v>
+        <v>0.121206589095398</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n"/>
       <c r="B117" s="1" t="inlineStr">
         <is>
-          <t>RES_WIND</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>12799.99992510269</v>
+        <v>888.9447563375129</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n"/>
       <c r="B118" s="1" t="inlineStr">
         <is>
-          <t>RES_SOLAR</t>
+          <t>BIOETHANOL</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>156424.75746334</v>
+        <v>0.07998521464824355</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n"/>
       <c r="B119" s="1" t="inlineStr">
         <is>
-          <t>RES_HYDRO</t>
+          <t>BIODIESEL</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>66970.63168393266</v>
+        <v>0.2254123025847234</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n"/>
       <c r="B120" s="1" t="inlineStr">
         <is>
-          <t>RES_GEO</t>
+          <t>LFO</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>2.201385642443737e-05</v>
+        <v>0.4912217960676011</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n"/>
       <c r="B121" s="1" t="inlineStr">
         <is>
-          <t>CO2_ATM</t>
+          <t>GAS</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>2.339076395621587e-05</v>
+        <v>0.6179238463046977</v>
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="1" t="inlineStr">
-        <is>
-          <t>YEAR_2045</t>
-        </is>
-      </c>
+      <c r="A122" s="1" t="n"/>
       <c r="B122" s="1" t="inlineStr">
         <is>
-          <t>ELECTRICITY</t>
+          <t>GAS_RE</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>1.429074037876386e-05</v>
+        <v>0.01071012823379835</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n"/>
       <c r="B123" s="1" t="inlineStr">
         <is>
-          <t>GASOLINE</t>
+          <t>WOOD</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>1.874792380767839e-05</v>
+        <v>74225.26906431503</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n"/>
       <c r="B124" s="1" t="inlineStr">
         <is>
-          <t>DIESEL</t>
+          <t>WET_BIOMASS</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>889.105859979543</v>
+        <v>49781.93825904865</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n"/>
       <c r="B125" s="1" t="inlineStr">
         <is>
-          <t>BIOETHANOL</t>
+          <t>COAL</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>1.732860155127214e-05</v>
+        <v>12307.85718288948</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n"/>
       <c r="B126" s="1" t="inlineStr">
         <is>
-          <t>BIODIESEL</t>
+          <t>WASTE</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>5.103445151680727e-05</v>
+        <v>2.039239488221757</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n"/>
       <c r="B127" s="1" t="inlineStr">
         <is>
-          <t>LFO</t>
+          <t>H2</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>0.0001081878842429957</v>
+        <v>0.008148066900239267</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n"/>
       <c r="B128" s="1" t="inlineStr">
         <is>
-          <t>GAS</t>
+          <t>H2_RE</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>8.073102851942465e-05</v>
+        <v>0.008286545616282105</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n"/>
       <c r="B129" s="1" t="inlineStr">
         <is>
-          <t>GAS_RE</t>
+          <t>AMMONIA_RE</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>3.008740670718074e-06</v>
+        <v>0.1503800677410024</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n"/>
       <c r="B130" s="1" t="inlineStr">
         <is>
-          <t>WOOD</t>
+          <t>METHANOL_RE</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>74227.5828966329</v>
+        <v>0.1309476232528584</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n"/>
       <c r="B131" s="1" t="inlineStr">
         <is>
-          <t>WET_BIOMASS</t>
+          <t>ELEC_EXPORT</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>49781.99997988063</v>
+        <v>2584.598469609186</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n"/>
       <c r="B132" s="1" t="inlineStr">
         <is>
-          <t>COAL</t>
+          <t>CO2_EMISSIONS</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>13277.8395244373</v>
+        <v>24287.40696079084</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n"/>
       <c r="B133" s="1" t="inlineStr">
         <is>
-          <t>WASTE</t>
+          <t>RES_WIND</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>0.0004701172403961716</v>
+        <v>2.914403489248679</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n"/>
       <c r="B134" s="1" t="inlineStr">
         <is>
-          <t>H2</t>
+          <t>RES_SOLAR</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>1.506261578684026e-06</v>
+        <v>328027.5892894726</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n"/>
       <c r="B135" s="1" t="inlineStr">
         <is>
-          <t>H2_RE</t>
+          <t>RES_HYDRO</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>1.356075686077731e-06</v>
+        <v>66230.70220803267</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n"/>
       <c r="B136" s="1" t="inlineStr">
         <is>
-          <t>AMMONIA_RE</t>
+          <t>RES_GEO</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>2.711143693743998e-05</v>
+        <v>0.1879588201768704</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n"/>
       <c r="B137" s="1" t="inlineStr">
         <is>
-          <t>METHANOL_RE</t>
+          <t>CO2_ATM</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2.565615412334167e-05</v>
+        <v>0.1867199140697204</v>
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="1" t="n"/>
+      <c r="A138" s="1" t="inlineStr">
+        <is>
+          <t>YEAR_2050</t>
+        </is>
+      </c>
       <c r="B138" s="1" t="inlineStr">
         <is>
-          <t>ELEC_EXPORT</t>
+          <t>ELECTRICITY</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>1879.832377317934</v>
+        <v>0.1172599036795307</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n"/>
       <c r="B139" s="1" t="inlineStr">
         <is>
-          <t>CO2_EMISSIONS</t>
+          <t>GASOLINE</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>26502.30674114201</v>
+        <v>0.1215301769247456</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n"/>
       <c r="B140" s="1" t="inlineStr">
         <is>
-          <t>RES_WIND</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>11753.54936792742</v>
+        <v>863.8724605778808</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n"/>
       <c r="B141" s="1" t="inlineStr">
         <is>
-          <t>RES_SOLAR</t>
+          <t>BIOETHANOL</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>300759.4934970301</v>
+        <v>0.250562275802667</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n"/>
       <c r="B142" s="1" t="inlineStr">
         <is>
-          <t>RES_HYDRO</t>
+          <t>BIODIESEL</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>66432.88090757444</v>
+        <v>0.8098101388760438</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n"/>
       <c r="B143" s="1" t="inlineStr">
         <is>
-          <t>RES_GEO</t>
+          <t>LFO</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>3.758641172211646e-05</v>
+        <v>0.3142644316047766</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n"/>
       <c r="B144" s="1" t="inlineStr">
         <is>
-          <t>CO2_ATM</t>
+          <t>GAS</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>4.09904363820519e-05</v>
+        <v>0.03437525726149267</v>
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="1" t="inlineStr">
-        <is>
-          <t>YEAR_2050</t>
-        </is>
-      </c>
+      <c r="A145" s="1" t="n"/>
       <c r="B145" s="1" t="inlineStr">
         <is>
-          <t>ELECTRICITY</t>
+          <t>GAS_RE</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>2.903557371175934e-05</v>
+        <v>0.1784322165938813</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n"/>
       <c r="B146" s="1" t="inlineStr">
         <is>
-          <t>GASOLINE</t>
+          <t>WOOD</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>3.565855273182939e-05</v>
+        <v>31127.89628047712</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n"/>
       <c r="B147" s="1" t="inlineStr">
         <is>
-          <t>DIESEL</t>
+          <t>WET_BIOMASS</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>864.9727302872974</v>
+        <v>49781.87480499965</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n"/>
       <c r="B148" s="1" t="inlineStr">
         <is>
-          <t>BIOETHANOL</t>
+          <t>COAL</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>3.774561126016488e-05</v>
+        <v>679.997672575314</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n"/>
       <c r="B149" s="1" t="inlineStr">
         <is>
-          <t>BIODIESEL</t>
+          <t>WASTE</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>0.0002617801153816169</v>
+        <v>1.805789363758634</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n"/>
       <c r="B150" s="1" t="inlineStr">
         <is>
-          <t>LFO</t>
+          <t>H2</t>
         </is>
       </c>
       <c r="C150" t="n">
-        <v>0.0001178340845070863</v>
+        <v>0.009046491669600136</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n"/>
       <c r="B151" s="1" t="inlineStr">
         <is>
-          <t>GAS</t>
+          <t>H2_RE</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>1.330100247628063e-05</v>
+        <v>0.01901808596926245</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n"/>
       <c r="B152" s="1" t="inlineStr">
         <is>
-          <t>GAS_RE</t>
+          <t>AMMONIA_RE</t>
         </is>
       </c>
       <c r="C152" t="n">
-        <v>9.80392710054608e-06</v>
+        <v>0.291980399490782</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n"/>
       <c r="B153" s="1" t="inlineStr">
         <is>
-          <t>WOOD</t>
+          <t>METHANOL_RE</t>
         </is>
       </c>
       <c r="C153" t="n">
-        <v>26874.50502348578</v>
+        <v>0.2351927634665876</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n"/>
       <c r="B154" s="1" t="inlineStr">
         <is>
-          <t>WET_BIOMASS</t>
+          <t>ELEC_EXPORT</t>
         </is>
       </c>
       <c r="C154" t="n">
-        <v>49781.99997256562</v>
+        <v>6367.459414439702</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n"/>
       <c r="B155" s="1" t="inlineStr">
         <is>
-          <t>COAL</t>
+          <t>CO2_EMISSIONS</t>
         </is>
       </c>
       <c r="C155" t="n">
-        <v>805.0813720749589</v>
+        <v>1.692786997423635</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n"/>
       <c r="B156" s="1" t="inlineStr">
         <is>
-          <t>WASTE</t>
+          <t>RES_WIND</t>
         </is>
       </c>
       <c r="C156" t="n">
-        <v>0.0006503363823748503</v>
+        <v>2.173083090764573</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n"/>
       <c r="B157" s="1" t="inlineStr">
         <is>
-          <t>H2</t>
+          <t>RES_SOLAR</t>
         </is>
       </c>
       <c r="C157" t="n">
-        <v>3.054550733365308e-06</v>
+        <v>412844.0977511517</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n"/>
       <c r="B158" s="1" t="inlineStr">
         <is>
-          <t>H2_RE</t>
+          <t>RES_HYDRO</t>
         </is>
       </c>
       <c r="C158" t="n">
-        <v>3.153626666848776e-06</v>
+        <v>65760.81559415076</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n"/>
       <c r="B159" s="1" t="inlineStr">
         <is>
-          <t>AMMONIA_RE</t>
+          <t>RES_GEO</t>
         </is>
       </c>
       <c r="C159" t="n">
-        <v>5.72961993704415e-05</v>
+        <v>0.5336367033908326</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n"/>
       <c r="B160" s="1" t="inlineStr">
         <is>
-          <t>METHANOL_RE</t>
+          <t>CO2_ATM</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>5.02351755637758e-05</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" s="1" t="n"/>
-      <c r="B161" s="1" t="inlineStr">
-        <is>
-          <t>ELEC_EXPORT</t>
-        </is>
-      </c>
-      <c r="C161" t="n">
-        <v>5753.153580667536</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" s="1" t="n"/>
-      <c r="B162" s="1" t="inlineStr">
-        <is>
-          <t>CO2_EMISSIONS</t>
-        </is>
-      </c>
-      <c r="C162" t="n">
-        <v>0.0002206624069174268</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" s="1" t="n"/>
-      <c r="B163" s="1" t="inlineStr">
-        <is>
-          <t>RES_WIND</t>
-        </is>
-      </c>
-      <c r="C163" t="n">
-        <v>0.0005523634253292436</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" s="1" t="n"/>
-      <c r="B164" s="1" t="inlineStr">
-        <is>
-          <t>RES_SOLAR</t>
-        </is>
-      </c>
-      <c r="C164" t="n">
-        <v>402885.3280069758</v>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" s="1" t="n"/>
-      <c r="B165" s="1" t="inlineStr">
-        <is>
-          <t>RES_HYDRO</t>
-        </is>
-      </c>
-      <c r="C165" t="n">
-        <v>65836.95736246253</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" s="1" t="n"/>
-      <c r="B166" s="1" t="inlineStr">
-        <is>
-          <t>RES_GEO</t>
-        </is>
-      </c>
-      <c r="C166" t="n">
-        <v>0.0001115679819965497</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" s="1" t="n"/>
-      <c r="B167" s="1" t="inlineStr">
-        <is>
-          <t>CO2_ATM</t>
-        </is>
-      </c>
-      <c r="C167" t="n">
-        <v>0.0003321291562130348</v>
+        <v>0.9320562971273568</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A145:A167"/>
-    <mergeCell ref="A122:A144"/>
-    <mergeCell ref="A2:A24"/>
-    <mergeCell ref="A25:A49"/>
-    <mergeCell ref="A74:A97"/>
-    <mergeCell ref="A50:A73"/>
-    <mergeCell ref="A98:A121"/>
+    <mergeCell ref="A67:A90"/>
+    <mergeCell ref="A43:A66"/>
+    <mergeCell ref="A91:A114"/>
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="A115:A137"/>
+    <mergeCell ref="A138:A160"/>
+    <mergeCell ref="A18:A42"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>